<commit_message>
Locator Challange with logs output
</commit_message>
<xml_diff>
--- a/Autosphere/Locator/Locator-Output.xlsx
+++ b/Autosphere/Locator/Locator-Output.xlsx
@@ -6,12 +6,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Germany" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mexico" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Netherlands" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="New Zealand" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nigeria" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Russia" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Australia" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="China" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="India" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="South Korea" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -429,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,43 +450,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ANDHRA PRADESH GRAMEENA VIKAS BANK</t>
+          <t>McDonalds</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PUNJAB NATIONAL BANK</t>
+          <t>Novartis</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CHAITANYA GODAVARI GRAMEENA BANK</t>
+          <t>MARUTHI SUZUKI</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PUNJAB &amp; SIND BANK</t>
+          <t>HYUNDAI</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -500,228 +498,492 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ARUNACHAL PRADESH RURAL BANK</t>
+          <t>NISSAN</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MAHARASHTRA GRAMIN BANK</t>
+          <t>MAHINDRA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CENTRAL BANK OF INDIA</t>
+          <t>SCODA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>UCO BANK</t>
+          <t>RENAULT</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ANDRA PRAGHATHI GRAMEENA BANK</t>
+          <t>BMW</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CANARA BANK</t>
+          <t>ROLLS ROYCE</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>INDIAN BANK</t>
+          <t>LAND ROVER</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>STATE BANK OF INDIA</t>
+          <t>BENZ</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BANK OF MAHARASHTRA</t>
+          <t>KIA</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MEGHALAYA RURAL BANK</t>
+          <t>STATE BANK OF INDIA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MADHYANCHAL GRAMIN BANK</t>
+          <t>BANK OF BARODA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BANK OF INDIA</t>
+          <t>BANK OF MAHARASHTRA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>NAGALAND RURAL BANK</t>
+          <t>CANARA BANK</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MIZORAM RURAL BANK</t>
+          <t>ANDRA PRAGHATHI GRAMEENA BANK</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>INDIAN OVERSEAS BANK</t>
+          <t>BANK OF INDIA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MANIPUR RURAL BANK</t>
+          <t>CENTRAL BANK OF INDIA</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LAND ROVER</t>
+          <t>INDIAN BANK</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SCODA</t>
+          <t>PUNJAB NATIONAL BANK</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>RENAULT</t>
+          <t>PUNJAB &amp; SIND BANK</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>UCO BANK</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ANDHRA PRADESH GRAMEENA VIKAS BANK</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CHAITANYA GODAVARI GRAMEENA BANK</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ARYAVART BANK</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ASSAM GRAMIN VIKASH BANK</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BARODA GUJARAT GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>BARODA RAJASTHAN KSHETRIYA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>BARODA UP BANK</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CHHATTISGARH RAJYA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ELLAQUAI DEHATI BANK</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>HIMACHAL PRADESH GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>J &amp; K GRAMEEN BANK</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>JHARKHAND RAJYA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>KARNATAKA VIKAS GRAMEENA BANK</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>MADHYA PRADESH GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>MADHYANCHAL GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>MAHARASHTRA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>MANIPUR RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>MEGHALAYA RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>MIZORAM RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>NAGALAND RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Origin Energy</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -736,7 +998,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -759,151 +1021,151 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ANDHRA PRADESH GRAMEENA VIKAS BANK</t>
+          <t>FORD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PUNJAB NATIONAL BANK</t>
+          <t>MARUTHI SUZUKI</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CHAITANYA GODAVARI GRAMEENA BANK</t>
+          <t>HYUNDAI</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ARUNACHAL PRADESH RURAL BANK</t>
+          <t>NISSAN</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MAHARASHTRA GRAMIN BANK</t>
+          <t>MAHINDRA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CENTRAL BANK OF INDIA</t>
+          <t>SCODA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ANDRA PRAGHATHI GRAMEENA BANK</t>
+          <t>BMW</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>UNION BANK OF INDIA</t>
+          <t>ROLLS ROYCE</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CANARA BANK</t>
+          <t>LAND ROVER</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>INDIAN BANK</t>
+          <t>BENZ</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>STATE BANK OF INDIA</t>
+          <t>KIA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BANK OF MAHARASHTRA</t>
+          <t>UNION BANK OF INDIA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MEGHALAYA RURAL BANK</t>
+          <t>STATE BANK OF INDIA</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -915,94 +1177,406 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MADHYANCHAL GRAMIN BANK</t>
+          <t>BANK OF BARODA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BANK OF INDIA</t>
+          <t>BANK OF MAHARASHTRA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>NAGALAND RURAL BANK</t>
+          <t>CANARA BANK</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MIZORAM RURAL BANK</t>
+          <t>ANDRA PRAGHATHI GRAMEENA BANK</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MANIPUR RURAL BANK</t>
+          <t>BANK OF INDIA</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LAND ROVER</t>
+          <t>CENTRAL BANK OF INDIA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SCODA</t>
+          <t>INDIAN BANK</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>RENAULT</t>
+          <t>INDIAN OVERSEAS BANK</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PUNJAB NATIONAL BANK</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PUNJAB &amp; SIND BANK</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>UCO BANK</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ANDHRA PRADESH GRAMEENA VIKAS BANK</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CHAITANYA GODAVARI GRAMEENA BANK</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ARUNACHAL PRADESH RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ARYAVART BANK</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BANGIYA GRAMIN VIKASH BANK</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>BARODA GUJARAT GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>BARODA RAJASTHAN KSHETRIYA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BARODA UP BANK</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CHHATTISGARH RAJYA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>DAKSHIN BIHAR GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>ELLAQUAI DEHATI BANK</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>HIMACHAL PRADESH GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>J &amp; K GRAMEEN BANK</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>JHARKHAND RAJYA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>KARNATAKA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>KARNATAKA VIKAS GRAMEENA BANK</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>KERALA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>MADHYA PRADESH GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>MADHYANCHAL GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>MANIPUR RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>MEGHALAYA RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>MIZORAM RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>NAGALAND RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -1019,7 +1593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1042,127 +1616,127 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ANDHRA PRADESH GRAMEENA VIKAS BANK</t>
+          <t>ICICI PRUDENTIAL</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PUNJAB NATIONAL BANK</t>
+          <t>MARUTHI SUZUKI</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CHAITANYA GODAVARI GRAMEENA BANK</t>
+          <t>HYUNDAI</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PUNJAB &amp; SIND BANK</t>
+          <t>NISSAN</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ARUNACHAL PRADESH RURAL BANK</t>
+          <t>SCODA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CENTRAL BANK OF INDIA</t>
+          <t>RENAULT</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>UCO BANK</t>
+          <t>ROLLS ROYCE</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ANDRA PRAGHATHI GRAMEENA BANK</t>
+          <t>BENZ</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>UNION BANK OF INDIA</t>
+          <t>KIA</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CANARA BANK</t>
+          <t>UNION BANK OF INDIA</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>INDIAN BANK</t>
+          <t>STATE BANK OF INDIA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1179,67 +1753,67 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>STATE BANK OF INDIA</t>
+          <t>BANK OF MAHARASHTRA</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BANK OF MAHARASHTRA</t>
+          <t>CANARA BANK</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MADHYANCHAL GRAMIN BANK</t>
+          <t>ANDRA PRAGHATHI GRAMEENA BANK</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BANK OF INDIA</t>
+          <t>CENTRAL BANK OF INDIA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MIZORAM RURAL BANK</t>
+          <t>INDIAN BANK</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -1251,55 +1825,295 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MANIPUR RURAL BANK</t>
+          <t>PUNJAB NATIONAL BANK</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LAND ROVER</t>
+          <t>PUNJAB &amp; SIND BANK</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SCODA</t>
+          <t>UCO BANK</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>RENAULT</t>
+          <t>ANDHRA PRADESH GRAMEENA VIKAS BANK</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ARUNACHAL PRADESH RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ARYAVART BANK</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ASSAM GRAMIN VIKASH BANK</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>BANGIYA GRAMIN VIKASH BANK</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>BARODA GUJARAT GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>BARODA UP BANK</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>DAKSHIN BIHAR GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>HIMACHAL PRADESH GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>J &amp; K GRAMEEN BANK</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>JHARKHAND RAJYA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>KARNATAKA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>KARNATAKA VIKAS GRAMEENA BANK</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>KERALA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>MADHYA PRADESH GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>MADHYANCHAL GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>MAHARASHTRA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>MANIPUR RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>MEGHALAYA RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>MIZORAM RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>NAGALAND RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1314,7 +2128,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1337,43 +2151,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ANDHRA PRADESH GRAMEENA VIKAS BANK</t>
+          <t>Kimberly Clark</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PUNJAB NATIONAL BANK</t>
+          <t>HYUNDAI</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CHAITANYA GODAVARI GRAMEENA BANK</t>
+          <t>MAHINDRA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PUNJAB &amp; SIND BANK</t>
+          <t>SCODA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1385,60 +2199,60 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ARUNACHAL PRADESH RURAL BANK</t>
+          <t>RENAULT</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MAHARASHTRA GRAMIN BANK</t>
+          <t>BMW</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CENTRAL BANK OF INDIA</t>
+          <t>ROLLS ROYCE</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>UCO BANK</t>
+          <t>LAND ROVER</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ANDRA PRAGHATHI GRAMEENA BANK</t>
+          <t>BENZ</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1450,55 +2264,55 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CANARA BANK</t>
+          <t>BANK OF BARODA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>INDIAN BANK</t>
+          <t>BANK OF MAHARASHTRA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>STATE BANK OF INDIA</t>
+          <t>CANARA BANK</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MEGHALAYA RURAL BANK</t>
+          <t>ANDRA PRAGHATHI GRAMEENA BANK</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -1517,686 +2331,312 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>NAGALAND RURAL BANK</t>
+          <t>CENTRAL BANK OF INDIA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MIZORAM RURAL BANK</t>
+          <t>INDIAN OVERSEAS BANK</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>INDIAN OVERSEAS BANK</t>
+          <t>PUNJAB NATIONAL BANK</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MANIPUR RURAL BANK</t>
+          <t>UCO BANK</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LAND ROVER</t>
+          <t>ANDHRA PRADESH GRAMEENA VIKAS BANK</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SCODA</t>
+          <t>CHAITANYA GODAVARI GRAMEENA BANK</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>CustomerName</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Number of Locations</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ANDHRA PRADESH GRAMEENA VIKAS BANK</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CHAITANYA GODAVARI GRAMEENA BANK</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>PUNJAB &amp; SIND BANK</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ARUNACHAL PRADESH RURAL BANK</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>MAHARASHTRA GRAMIN BANK</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>CENTRAL BANK OF INDIA</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>UCO BANK</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>ANDRA PRAGHATHI GRAMEENA BANK</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>UNION BANK OF INDIA</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>CANARA BANK</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>INDIAN BANK</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>BANK OF BARODA</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>STATE BANK OF INDIA</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>BANK OF MAHARASHTRA</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>MEGHALAYA RURAL BANK</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>MADHYANCHAL GRAMIN BANK</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>NAGALAND RURAL BANK</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>MIZORAM RURAL BANK</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>INDIAN OVERSEAS BANK</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>MANIPUR RURAL BANK</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LAND ROVER</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SCODA</t>
+          <t>ARUNACHAL PRADESH RURAL BANK</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>RENAULT</t>
+          <t>ARYAVART BANK</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ASSAM GRAMIN VIKASH BANK</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>BANGIYA GRAMIN VIKASH BANK</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>BARODA RAJASTHAN KSHETRIYA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>BARODA UP BANK</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>CustomerName</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Number of Locations</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ANDHRA PRADESH GRAMEENA VIKAS BANK</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CHHATTISGARH RAJYA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>DAKSHIN BIHAR GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ELLAQUAI DEHATI BANK</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>HIMACHAL PRADESH GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>JHARKHAND RAJYA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>KARNATAKA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>KARNATAKA VIKAS GRAMEENA BANK</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>KERALA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>MADHYA PRADESH GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>MADHYANCHAL GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>PUNJAB NATIONAL BANK</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>MAHARASHTRA GRAMIN BANK</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>MANIPUR RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>MEGHALAYA RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>NAGALAND RURAL BANK</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>9</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CHAITANYA GODAVARI GRAMEENA BANK</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>PUNJAB &amp; SIND BANK</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ARUNACHAL PRADESH RURAL BANK</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>MAHARASHTRA GRAMIN BANK</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>CENTRAL BANK OF INDIA</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>UCO BANK</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ANDRA PRAGHATHI GRAMEENA BANK</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>UNION BANK OF INDIA</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>CANARA BANK</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>INDIAN BANK</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>BANK OF BARODA</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>STATE BANK OF INDIA</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>BANK OF MAHARASHTRA</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>MADHYANCHAL GRAMIN BANK</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>BANK OF INDIA</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>MIZORAM RURAL BANK</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>INDIAN OVERSEAS BANK</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>MANIPUR RURAL BANK</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LAND ROVER</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>SCODA</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>RENAULT</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>